<commit_message>
jn: dominios de valores e informes casi finales jn
</commit_message>
<xml_diff>
--- a/05_Entregable 3/previo/Diccionarios/MD_03_MAATE_BD_2021_VS (1).xlsx
+++ b/05_Entregable 3/previo/Diccionarios/MD_03_MAATE_BD_2021_VS (1).xlsx
@@ -1,15 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
-  <fileVersion appName="xl" lastEdited="6" lowestEdited="7" rupBuild="14420"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="28623"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Disco_F\!!Personal\Mio\1_WCS 2024\wcs\05_Entregable 3\previo\Diccionarios\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="F:\Javi_Angelito\wcs\05_Entregable 3\previo\Diccionarios\"/>
     </mc:Choice>
   </mc:AlternateContent>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B2B2106A-6A4A-4405-86F5-80EA1AC56A93}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" firstSheet="2" activeTab="4"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Metadatos generales" sheetId="1" r:id="rId1"/>
@@ -43,9 +44,6 @@
   </si>
   <si>
     <t>Versión</t>
-  </si>
-  <si>
-    <t>1.0</t>
   </si>
   <si>
     <t>Fecha de creación</t>
@@ -702,18 +700,6 @@
     <t>hora_retencion</t>
   </si>
   <si>
-    <t>coord_x_rescate</t>
-  </si>
-  <si>
-    <t>coord_y_rescate</t>
-  </si>
-  <si>
-    <t>coord_x_retencion</t>
-  </si>
-  <si>
-    <t>coord_y_retencion</t>
-  </si>
-  <si>
     <t>apellidos_retencion</t>
   </si>
   <si>
@@ -779,11 +765,26 @@
   <si>
     <t>Costo monetario en USD asociado a los especímenes retenidos</t>
   </si>
+  <si>
+    <t>2.0</t>
+  </si>
+  <si>
+    <t>longitud_rescate</t>
+  </si>
+  <si>
+    <t>latitud_rescate</t>
+  </si>
+  <si>
+    <t>latitud_retencion</t>
+  </si>
+  <si>
+    <t>longitud_retencion</t>
+  </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
   <fonts count="5" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
@@ -874,7 +875,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="20">
+  <cellXfs count="18">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
@@ -902,11 +903,9 @@
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="4" fillId="2" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="3" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
     <xf numFmtId="0" fontId="2" fillId="4" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -1121,10 +1120,12 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A2:B1000"/>
   <sheetViews>
-    <sheetView workbookViewId="0"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="B5" sqref="B5"/>
+    </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="14.42578125" defaultRowHeight="15" customHeight="1" x14ac:dyDescent="0.25"/>
   <cols>
@@ -1154,31 +1155,31 @@
         <v>4</v>
       </c>
       <c r="B4" s="5" t="s">
-        <v>5</v>
+        <v>245</v>
       </c>
     </row>
     <row r="5" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A5" s="3" t="s">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="B5" s="6">
-        <v>45721</v>
+        <v>45782</v>
       </c>
     </row>
     <row r="6" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A6" s="3" t="s">
+        <v>6</v>
+      </c>
+      <c r="B6" s="4" t="s">
         <v>7</v>
-      </c>
-      <c r="B6" s="4" t="s">
-        <v>8</v>
       </c>
     </row>
     <row r="7" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A7" s="3" t="s">
+        <v>8</v>
+      </c>
+      <c r="B7" s="4" t="s">
         <v>9</v>
-      </c>
-      <c r="B7" s="4" t="s">
-        <v>10</v>
       </c>
     </row>
     <row r="21" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
@@ -2168,7 +2169,7 @@
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
   <dimension ref="A1:C1000"/>
   <sheetViews>
     <sheetView workbookViewId="0"/>
@@ -2183,64 +2184,64 @@
   <sheetData>
     <row r="1" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A1" s="7" t="s">
+        <v>10</v>
+      </c>
+      <c r="B1" s="7" t="s">
         <v>11</v>
-      </c>
-      <c r="B1" s="7" t="s">
-        <v>12</v>
       </c>
     </row>
     <row r="2" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A2" s="7" t="s">
+        <v>12</v>
+      </c>
+      <c r="B2" s="7" t="s">
         <v>13</v>
-      </c>
-      <c r="B2" s="7" t="s">
-        <v>14</v>
       </c>
     </row>
     <row r="3" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A3" s="7" t="s">
+        <v>14</v>
+      </c>
+      <c r="B3" s="7" t="s">
         <v>15</v>
-      </c>
-      <c r="B3" s="7" t="s">
-        <v>16</v>
       </c>
     </row>
     <row r="4" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A4" s="7" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
     </row>
     <row r="5" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A5" s="7" t="s">
+        <v>17</v>
+      </c>
+      <c r="B5" s="7" t="s">
         <v>18</v>
-      </c>
-      <c r="B5" s="7" t="s">
-        <v>19</v>
       </c>
     </row>
     <row r="6" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A6" s="7" t="s">
+        <v>19</v>
+      </c>
+      <c r="B6" s="7" t="s">
         <v>20</v>
-      </c>
-      <c r="B6" s="7" t="s">
-        <v>21</v>
       </c>
     </row>
     <row r="7" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A7" s="7" t="s">
+        <v>21</v>
+      </c>
+      <c r="B7" s="8" t="s">
         <v>22</v>
-      </c>
-      <c r="B7" s="8" t="s">
-        <v>23</v>
       </c>
       <c r="C7" s="9"/>
     </row>
     <row r="8" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A8" s="7" t="s">
+        <v>23</v>
+      </c>
+      <c r="B8" s="10" t="s">
         <v>24</v>
-      </c>
-      <c r="B8" s="10" t="s">
-        <v>25</v>
       </c>
     </row>
     <row r="21" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
@@ -3230,12 +3231,12 @@
 </file>
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0200-000000000000}">
   <dimension ref="A1:Z1000"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <pane xSplit="1" topLeftCell="G1" activePane="topRight" state="frozen"/>
-      <selection pane="topRight" activeCell="H19" sqref="H19"/>
+      <pane xSplit="1" topLeftCell="B1" activePane="topRight" state="frozen"/>
+      <selection pane="topRight" activeCell="B6" sqref="B6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="14.42578125" defaultRowHeight="15" customHeight="1" x14ac:dyDescent="0.25"/>
@@ -3252,410 +3253,410 @@
   <sheetData>
     <row r="1" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A1" s="11" t="s">
+        <v>196</v>
+      </c>
+      <c r="B1" s="11" t="s">
         <v>197</v>
       </c>
-      <c r="B1" s="11" t="s">
-        <v>198</v>
-      </c>
       <c r="C1" s="11" t="s">
+        <v>25</v>
+      </c>
+      <c r="D1" s="11" t="s">
         <v>26</v>
       </c>
-      <c r="D1" s="11" t="s">
+      <c r="E1" s="11" t="s">
         <v>27</v>
       </c>
-      <c r="E1" s="11" t="s">
+      <c r="F1" s="11" t="s">
         <v>28</v>
       </c>
-      <c r="F1" s="11" t="s">
+      <c r="G1" s="11" t="s">
         <v>29</v>
       </c>
-      <c r="G1" s="11" t="s">
+      <c r="H1" s="11" t="s">
         <v>30</v>
       </c>
-      <c r="H1" s="11" t="s">
-        <v>31</v>
-      </c>
       <c r="I1" s="11" t="s">
-        <v>219</v>
+        <v>218</v>
       </c>
     </row>
     <row r="2" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A2" s="7" t="s">
+        <v>31</v>
+      </c>
+      <c r="B2" t="s">
+        <v>198</v>
+      </c>
+      <c r="C2" s="12" t="s">
         <v>32</v>
       </c>
-      <c r="B2" s="15" t="s">
-        <v>199</v>
-      </c>
-      <c r="C2" s="12" t="s">
+      <c r="D2" s="12" t="s">
         <v>33</v>
       </c>
-      <c r="D2" s="12" t="s">
+      <c r="E2" s="12" t="s">
         <v>34</v>
       </c>
-      <c r="E2" s="12" t="s">
+      <c r="F2" s="12" t="s">
         <v>35</v>
       </c>
-      <c r="F2" s="12" t="s">
+      <c r="G2" s="12" t="s">
         <v>36</v>
-      </c>
-      <c r="G2" s="12" t="s">
-        <v>37</v>
       </c>
       <c r="H2" s="12"/>
     </row>
     <row r="3" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A3" s="13" t="s">
+        <v>37</v>
+      </c>
+      <c r="B3" s="13" t="s">
+        <v>199</v>
+      </c>
+      <c r="C3" s="12" t="s">
         <v>38</v>
       </c>
-      <c r="B3" s="13" t="s">
-        <v>200</v>
-      </c>
-      <c r="C3" s="12" t="s">
+      <c r="D3" s="12" t="s">
         <v>39</v>
       </c>
-      <c r="D3" s="12" t="s">
-        <v>40</v>
-      </c>
       <c r="E3" s="12" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
       <c r="F3" s="12" t="s">
         <v>1</v>
       </c>
       <c r="G3" s="12" t="s">
-        <v>41</v>
+        <v>40</v>
       </c>
       <c r="H3" s="12"/>
     </row>
     <row r="4" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A4" s="13" t="s">
+        <v>41</v>
+      </c>
+      <c r="B4" s="13" t="s">
+        <v>200</v>
+      </c>
+      <c r="C4" s="12" t="s">
         <v>42</v>
       </c>
-      <c r="B4" s="13" t="s">
-        <v>201</v>
-      </c>
-      <c r="C4" s="12" t="s">
-        <v>43</v>
-      </c>
       <c r="D4" s="12" t="s">
-        <v>40</v>
+        <v>39</v>
       </c>
       <c r="E4" s="12" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
       <c r="F4" s="12" t="s">
         <v>1</v>
       </c>
       <c r="G4" s="12" t="s">
-        <v>44</v>
+        <v>43</v>
       </c>
       <c r="H4" s="12"/>
     </row>
     <row r="5" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A5" s="13" t="s">
+        <v>44</v>
+      </c>
+      <c r="B5" s="13" t="s">
+        <v>247</v>
+      </c>
+      <c r="C5" s="12" t="s">
         <v>45</v>
       </c>
-      <c r="B5" s="13" t="s">
-        <v>224</v>
-      </c>
-      <c r="C5" s="12" t="s">
+      <c r="D5" s="12" t="s">
         <v>46</v>
       </c>
-      <c r="D5" s="12" t="s">
+      <c r="E5" s="12" t="s">
+        <v>34</v>
+      </c>
+      <c r="F5" s="12" t="s">
         <v>47</v>
       </c>
-      <c r="E5" s="12" t="s">
-        <v>35</v>
-      </c>
-      <c r="F5" s="12" t="s">
+      <c r="G5" s="12" t="s">
         <v>48</v>
       </c>
-      <c r="G5" s="12" t="s">
+      <c r="H5" s="12" t="s">
         <v>49</v>
-      </c>
-      <c r="H5" s="12" t="s">
-        <v>50</v>
       </c>
     </row>
     <row r="6" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A6" s="13" t="s">
+        <v>50</v>
+      </c>
+      <c r="B6" s="13" t="s">
+        <v>246</v>
+      </c>
+      <c r="C6" s="12" t="s">
         <v>51</v>
       </c>
-      <c r="B6" s="13" t="s">
-        <v>225</v>
-      </c>
-      <c r="C6" s="12" t="s">
+      <c r="D6" s="12" t="s">
+        <v>46</v>
+      </c>
+      <c r="E6" s="12" t="s">
+        <v>34</v>
+      </c>
+      <c r="F6" s="12" t="s">
+        <v>47</v>
+      </c>
+      <c r="G6" s="12" t="s">
         <v>52</v>
       </c>
-      <c r="D6" s="12" t="s">
-        <v>47</v>
-      </c>
-      <c r="E6" s="12" t="s">
-        <v>35</v>
-      </c>
-      <c r="F6" s="12" t="s">
-        <v>48</v>
-      </c>
-      <c r="G6" s="12" t="s">
-        <v>53</v>
-      </c>
       <c r="H6" s="12" t="s">
-        <v>50</v>
+        <v>49</v>
       </c>
     </row>
     <row r="7" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A7" s="13" t="s">
+        <v>53</v>
+      </c>
+      <c r="B7" s="13" t="s">
+        <v>242</v>
+      </c>
+      <c r="C7" s="12" t="s">
         <v>54</v>
       </c>
-      <c r="B7" s="13" t="s">
-        <v>247</v>
-      </c>
-      <c r="C7" s="12" t="s">
-        <v>55</v>
-      </c>
       <c r="D7" s="12" t="s">
+        <v>33</v>
+      </c>
+      <c r="E7" s="12" t="s">
         <v>34</v>
-      </c>
-      <c r="E7" s="12" t="s">
-        <v>35</v>
       </c>
       <c r="F7" s="12" t="s">
         <v>1</v>
       </c>
       <c r="G7" s="12" t="s">
+        <v>55</v>
+      </c>
+      <c r="H7" s="12" t="s">
         <v>56</v>
-      </c>
-      <c r="H7" s="12" t="s">
-        <v>57</v>
       </c>
     </row>
     <row r="8" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A8" s="13" t="s">
+        <v>57</v>
+      </c>
+      <c r="B8" s="13" t="s">
+        <v>201</v>
+      </c>
+      <c r="C8" s="12" t="s">
         <v>58</v>
       </c>
-      <c r="B8" s="13" t="s">
-        <v>202</v>
-      </c>
-      <c r="C8" s="12" t="s">
-        <v>59</v>
-      </c>
       <c r="D8" s="12" t="s">
+        <v>33</v>
+      </c>
+      <c r="E8" s="12" t="s">
         <v>34</v>
-      </c>
-      <c r="E8" s="12" t="s">
-        <v>35</v>
       </c>
       <c r="F8" s="12" t="s">
         <v>1</v>
       </c>
       <c r="G8" s="12" t="s">
-        <v>60</v>
+        <v>59</v>
       </c>
       <c r="H8" s="12" t="s">
-        <v>57</v>
+        <v>56</v>
       </c>
     </row>
     <row r="9" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A9" s="13" t="s">
+        <v>60</v>
+      </c>
+      <c r="B9" s="13" t="s">
+        <v>202</v>
+      </c>
+      <c r="C9" s="12" t="s">
         <v>61</v>
       </c>
-      <c r="B9" s="13" t="s">
-        <v>203</v>
-      </c>
-      <c r="C9" s="12" t="s">
-        <v>62</v>
-      </c>
       <c r="D9" s="12" t="s">
+        <v>33</v>
+      </c>
+      <c r="E9" s="12" t="s">
         <v>34</v>
-      </c>
-      <c r="E9" s="12" t="s">
-        <v>35</v>
       </c>
       <c r="F9" s="12" t="s">
         <v>1</v>
       </c>
       <c r="G9" s="12" t="s">
-        <v>63</v>
+        <v>62</v>
       </c>
       <c r="H9" s="12"/>
     </row>
     <row r="10" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A10" s="13" t="s">
+        <v>63</v>
+      </c>
+      <c r="B10" s="13" t="s">
+        <v>203</v>
+      </c>
+      <c r="C10" s="12" t="s">
         <v>64</v>
       </c>
-      <c r="B10" s="13" t="s">
-        <v>204</v>
-      </c>
-      <c r="C10" s="12" t="s">
-        <v>65</v>
-      </c>
       <c r="D10" s="12" t="s">
+        <v>33</v>
+      </c>
+      <c r="E10" s="12" t="s">
         <v>34</v>
-      </c>
-      <c r="E10" s="12" t="s">
-        <v>35</v>
       </c>
       <c r="F10" s="12" t="s">
         <v>1</v>
       </c>
       <c r="G10" s="12" t="s">
-        <v>66</v>
+        <v>65</v>
       </c>
       <c r="H10" s="12"/>
     </row>
     <row r="11" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A11" s="13" t="s">
+        <v>66</v>
+      </c>
+      <c r="B11" s="13" t="s">
+        <v>204</v>
+      </c>
+      <c r="C11" s="12" t="s">
         <v>67</v>
       </c>
-      <c r="B11" s="13" t="s">
-        <v>205</v>
-      </c>
-      <c r="C11" s="12" t="s">
-        <v>68</v>
-      </c>
       <c r="D11" s="12" t="s">
+        <v>33</v>
+      </c>
+      <c r="E11" s="12" t="s">
         <v>34</v>
-      </c>
-      <c r="E11" s="12" t="s">
-        <v>35</v>
       </c>
       <c r="F11" s="12" t="s">
         <v>1</v>
       </c>
       <c r="G11" s="12" t="s">
+        <v>68</v>
+      </c>
+      <c r="H11" s="12"/>
+    </row>
+    <row r="12" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A12" s="16" t="s">
         <v>69</v>
       </c>
-      <c r="H11" s="12"/>
-    </row>
-    <row r="12" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A12" s="17" t="s">
+      <c r="B12" s="13" t="s">
+        <v>205</v>
+      </c>
+      <c r="C12" s="12" t="s">
         <v>70</v>
       </c>
-      <c r="B12" s="13" t="s">
-        <v>206</v>
-      </c>
-      <c r="C12" s="12" t="s">
+      <c r="D12" s="12" t="s">
         <v>71</v>
       </c>
-      <c r="D12" s="12" t="s">
+      <c r="E12" s="14" t="s">
         <v>72</v>
-      </c>
-      <c r="E12" s="14" t="s">
-        <v>73</v>
       </c>
       <c r="F12" s="12" t="s">
         <v>1</v>
       </c>
       <c r="G12" s="12" t="s">
+        <v>73</v>
+      </c>
+      <c r="H12" s="12" t="s">
         <v>74</v>
       </c>
-      <c r="H12" s="12" t="s">
+      <c r="I12" s="12" t="s">
+        <v>219</v>
+      </c>
+    </row>
+    <row r="13" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A13" s="16" t="s">
         <v>75</v>
       </c>
-      <c r="I12" s="12" t="s">
-        <v>220</v>
-      </c>
-    </row>
-    <row r="13" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A13" s="17" t="s">
+      <c r="B13" s="13" t="s">
+        <v>206</v>
+      </c>
+      <c r="C13" s="12" t="s">
         <v>76</v>
       </c>
-      <c r="B13" s="13" t="s">
-        <v>207</v>
-      </c>
-      <c r="C13" s="12" t="s">
-        <v>77</v>
-      </c>
       <c r="D13" s="12" t="s">
+        <v>71</v>
+      </c>
+      <c r="E13" s="14" t="s">
         <v>72</v>
-      </c>
-      <c r="E13" s="14" t="s">
-        <v>73</v>
       </c>
       <c r="F13" s="12" t="s">
         <v>1</v>
       </c>
       <c r="G13" s="12" t="s">
+        <v>77</v>
+      </c>
+      <c r="H13" s="12" t="s">
+        <v>74</v>
+      </c>
+      <c r="I13" s="12" t="s">
+        <v>219</v>
+      </c>
+    </row>
+    <row r="14" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A14" s="16" t="s">
         <v>78</v>
       </c>
-      <c r="H13" s="12" t="s">
-        <v>75</v>
-      </c>
-      <c r="I13" s="12" t="s">
-        <v>220</v>
-      </c>
-    </row>
-    <row r="14" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A14" s="17" t="s">
+      <c r="B14" s="13" t="s">
+        <v>207</v>
+      </c>
+      <c r="C14" s="12" t="s">
         <v>79</v>
       </c>
-      <c r="B14" s="13" t="s">
-        <v>208</v>
-      </c>
-      <c r="C14" s="12" t="s">
-        <v>80</v>
-      </c>
       <c r="D14" s="12" t="s">
+        <v>71</v>
+      </c>
+      <c r="E14" s="14" t="s">
         <v>72</v>
-      </c>
-      <c r="E14" s="14" t="s">
-        <v>73</v>
       </c>
       <c r="F14" s="12" t="s">
         <v>1</v>
       </c>
       <c r="G14" s="12" t="s">
-        <v>81</v>
+        <v>80</v>
       </c>
       <c r="H14" s="12" t="s">
-        <v>75</v>
+        <v>74</v>
       </c>
       <c r="I14" s="12" t="s">
-        <v>220</v>
+        <v>219</v>
       </c>
     </row>
     <row r="15" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A15" s="13" t="s">
+        <v>81</v>
+      </c>
+      <c r="B15" s="13" t="s">
+        <v>208</v>
+      </c>
+      <c r="C15" s="12" t="s">
         <v>82</v>
       </c>
-      <c r="B15" s="13" t="s">
-        <v>209</v>
-      </c>
-      <c r="C15" s="12" t="s">
-        <v>83</v>
-      </c>
       <c r="D15" s="12" t="s">
+        <v>33</v>
+      </c>
+      <c r="E15" s="12" t="s">
         <v>34</v>
-      </c>
-      <c r="E15" s="12" t="s">
-        <v>35</v>
       </c>
       <c r="F15" s="12" t="s">
         <v>1</v>
       </c>
       <c r="G15" s="12" t="s">
-        <v>84</v>
+        <v>83</v>
       </c>
       <c r="H15" s="12"/>
     </row>
     <row r="16" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A16" s="13" t="s">
+        <v>84</v>
+      </c>
+      <c r="B16" s="13" t="s">
+        <v>209</v>
+      </c>
+      <c r="C16" s="12" t="s">
         <v>85</v>
       </c>
-      <c r="B16" s="13" t="s">
-        <v>210</v>
-      </c>
-      <c r="C16" s="12" t="s">
+      <c r="D16" s="12" t="s">
+        <v>46</v>
+      </c>
+      <c r="E16" s="12" t="s">
+        <v>34</v>
+      </c>
+      <c r="F16" s="12" t="s">
         <v>86</v>
-      </c>
-      <c r="D16" s="12" t="s">
-        <v>47</v>
-      </c>
-      <c r="E16" s="12" t="s">
-        <v>35</v>
-      </c>
-      <c r="F16" s="12" t="s">
-        <v>87</v>
       </c>
       <c r="G16" s="12">
         <v>1</v>
@@ -3664,22 +3665,22 @@
     </row>
     <row r="17" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A17" s="13" t="s">
+        <v>87</v>
+      </c>
+      <c r="B17" s="13" t="s">
+        <v>210</v>
+      </c>
+      <c r="C17" s="12" t="s">
         <v>88</v>
       </c>
-      <c r="B17" s="13" t="s">
-        <v>211</v>
-      </c>
-      <c r="C17" s="12" t="s">
-        <v>89</v>
-      </c>
       <c r="D17" s="12" t="s">
-        <v>47</v>
+        <v>46</v>
       </c>
       <c r="E17" s="12" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
       <c r="F17" s="12" t="s">
-        <v>87</v>
+        <v>86</v>
       </c>
       <c r="G17" s="12">
         <v>1</v>
@@ -3688,22 +3689,22 @@
     </row>
     <row r="18" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A18" s="13" t="s">
+        <v>89</v>
+      </c>
+      <c r="B18" s="13" t="s">
+        <v>211</v>
+      </c>
+      <c r="C18" s="12" t="s">
         <v>90</v>
       </c>
-      <c r="B18" s="13" t="s">
-        <v>212</v>
-      </c>
-      <c r="C18" s="12" t="s">
-        <v>91</v>
-      </c>
       <c r="D18" s="12" t="s">
-        <v>47</v>
+        <v>46</v>
       </c>
       <c r="E18" s="12" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
       <c r="F18" s="12" t="s">
-        <v>87</v>
+        <v>86</v>
       </c>
       <c r="G18" s="12">
         <v>2</v>
@@ -3711,226 +3712,226 @@
       <c r="H18" s="12"/>
     </row>
     <row r="19" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A19" s="17" t="s">
+      <c r="A19" s="16" t="s">
+        <v>91</v>
+      </c>
+      <c r="B19" s="13" t="s">
+        <v>212</v>
+      </c>
+      <c r="C19" s="12" t="s">
         <v>92</v>
       </c>
-      <c r="B19" s="13" t="s">
+      <c r="D19" s="12" t="s">
+        <v>71</v>
+      </c>
+      <c r="E19" s="14" t="s">
+        <v>72</v>
+      </c>
+      <c r="F19" s="12" t="s">
+        <v>86</v>
+      </c>
+      <c r="G19" s="12" t="s">
+        <v>93</v>
+      </c>
+      <c r="H19" s="12" t="s">
+        <v>74</v>
+      </c>
+    </row>
+    <row r="20" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A20" s="16" t="s">
+        <v>94</v>
+      </c>
+      <c r="B20" s="13" t="s">
         <v>213</v>
       </c>
-      <c r="C19" s="12" t="s">
-        <v>93</v>
-      </c>
-      <c r="D19" s="12" t="s">
+      <c r="C20" s="12" t="s">
+        <v>95</v>
+      </c>
+      <c r="D20" s="12" t="s">
+        <v>71</v>
+      </c>
+      <c r="E20" s="14" t="s">
         <v>72</v>
       </c>
-      <c r="E19" s="14" t="s">
-        <v>73</v>
-      </c>
-      <c r="F19" s="12" t="s">
-        <v>87</v>
-      </c>
-      <c r="G19" s="12" t="s">
-        <v>94</v>
-      </c>
-      <c r="H19" s="12" t="s">
-        <v>75</v>
-      </c>
-    </row>
-    <row r="20" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A20" s="17" t="s">
-        <v>95</v>
-      </c>
-      <c r="B20" s="13" t="s">
+      <c r="F20" s="12" t="s">
+        <v>86</v>
+      </c>
+      <c r="G20" s="12" t="s">
+        <v>96</v>
+      </c>
+      <c r="H20" s="12" t="s">
+        <v>74</v>
+      </c>
+    </row>
+    <row r="21" spans="1:8" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A21" s="16" t="s">
+        <v>97</v>
+      </c>
+      <c r="B21" s="13" t="s">
         <v>214</v>
       </c>
-      <c r="C20" s="12" t="s">
-        <v>96</v>
-      </c>
-      <c r="D20" s="12" t="s">
+      <c r="C21" s="12" t="s">
+        <v>98</v>
+      </c>
+      <c r="D21" s="12" t="s">
+        <v>71</v>
+      </c>
+      <c r="E21" s="14" t="s">
         <v>72</v>
-      </c>
-      <c r="E20" s="14" t="s">
-        <v>73</v>
-      </c>
-      <c r="F20" s="12" t="s">
-        <v>87</v>
-      </c>
-      <c r="G20" s="12" t="s">
-        <v>97</v>
-      </c>
-      <c r="H20" s="12" t="s">
-        <v>75</v>
-      </c>
-    </row>
-    <row r="21" spans="1:8" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A21" s="17" t="s">
-        <v>98</v>
-      </c>
-      <c r="B21" s="13" t="s">
-        <v>215</v>
-      </c>
-      <c r="C21" s="12" t="s">
-        <v>99</v>
-      </c>
-      <c r="D21" s="12" t="s">
-        <v>72</v>
-      </c>
-      <c r="E21" s="14" t="s">
-        <v>73</v>
       </c>
       <c r="F21" s="12" t="s">
         <v>1</v>
       </c>
       <c r="G21" s="12" t="s">
-        <v>100</v>
+        <v>99</v>
       </c>
       <c r="H21" s="12" t="s">
-        <v>75</v>
+        <v>74</v>
       </c>
     </row>
     <row r="22" spans="1:8" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A22" s="13" t="s">
+        <v>100</v>
+      </c>
+      <c r="B22" s="13" t="s">
+        <v>243</v>
+      </c>
+      <c r="C22" s="12" t="s">
         <v>101</v>
       </c>
-      <c r="B22" s="13" t="s">
-        <v>248</v>
-      </c>
-      <c r="C22" s="12" t="s">
-        <v>102</v>
-      </c>
       <c r="D22" s="12" t="s">
+        <v>33</v>
+      </c>
+      <c r="E22" s="12" t="s">
         <v>34</v>
-      </c>
-      <c r="E22" s="12" t="s">
-        <v>35</v>
       </c>
       <c r="F22" s="12" t="s">
         <v>1</v>
       </c>
       <c r="G22" s="12" t="s">
+        <v>102</v>
+      </c>
+      <c r="H22" s="12" t="s">
         <v>103</v>
-      </c>
-      <c r="H22" s="12" t="s">
-        <v>104</v>
       </c>
     </row>
     <row r="23" spans="1:8" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A23" s="13" t="s">
+        <v>104</v>
+      </c>
+      <c r="B23" s="13" t="s">
+        <v>215</v>
+      </c>
+      <c r="C23" s="12" t="s">
         <v>105</v>
       </c>
-      <c r="B23" s="13" t="s">
-        <v>216</v>
-      </c>
-      <c r="C23" s="12" t="s">
-        <v>106</v>
-      </c>
       <c r="D23" s="12" t="s">
+        <v>33</v>
+      </c>
+      <c r="E23" s="12" t="s">
         <v>34</v>
-      </c>
-      <c r="E23" s="12" t="s">
-        <v>35</v>
       </c>
       <c r="F23" s="12" t="s">
         <v>1</v>
       </c>
       <c r="G23" s="12" t="s">
-        <v>107</v>
+        <v>106</v>
       </c>
       <c r="H23" s="12" t="s">
-        <v>57</v>
+        <v>56</v>
       </c>
     </row>
     <row r="24" spans="1:8" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A24" s="13" t="s">
+        <v>107</v>
+      </c>
+      <c r="B24" s="13" t="s">
+        <v>216</v>
+      </c>
+      <c r="C24" s="12" t="s">
         <v>108</v>
       </c>
-      <c r="B24" s="13" t="s">
-        <v>217</v>
-      </c>
-      <c r="C24" s="12" t="s">
-        <v>109</v>
-      </c>
       <c r="D24" s="12" t="s">
-        <v>40</v>
+        <v>39</v>
       </c>
       <c r="E24" s="12" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
       <c r="F24" s="12" t="s">
         <v>1</v>
       </c>
       <c r="G24" s="12" t="s">
-        <v>110</v>
+        <v>109</v>
       </c>
       <c r="H24" s="12"/>
     </row>
     <row r="25" spans="1:8" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A25" s="13" t="s">
+        <v>110</v>
+      </c>
+      <c r="B25" s="13" t="s">
+        <v>217</v>
+      </c>
+      <c r="C25" s="12" t="s">
         <v>111</v>
       </c>
-      <c r="B25" s="13" t="s">
-        <v>218</v>
-      </c>
-      <c r="C25" s="12" t="s">
-        <v>112</v>
-      </c>
       <c r="D25" s="12" t="s">
+        <v>33</v>
+      </c>
+      <c r="E25" s="12" t="s">
         <v>34</v>
-      </c>
-      <c r="E25" s="12" t="s">
-        <v>35</v>
       </c>
       <c r="F25" s="12" t="s">
         <v>1</v>
       </c>
       <c r="G25" s="12" t="s">
-        <v>113</v>
+        <v>112</v>
       </c>
       <c r="H25" s="12"/>
     </row>
     <row r="26" spans="1:8" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A26" s="13" t="s">
+        <v>113</v>
+      </c>
+      <c r="B26" s="13" t="s">
+        <v>238</v>
+      </c>
+      <c r="C26" s="12" t="s">
         <v>114</v>
       </c>
-      <c r="B26" s="13" t="s">
-        <v>243</v>
-      </c>
-      <c r="C26" s="12" t="s">
-        <v>115</v>
-      </c>
       <c r="D26" s="12" t="s">
+        <v>33</v>
+      </c>
+      <c r="E26" s="12" t="s">
         <v>34</v>
-      </c>
-      <c r="E26" s="12" t="s">
-        <v>35</v>
       </c>
       <c r="F26" s="12" t="s">
         <v>1</v>
       </c>
       <c r="G26" s="12" t="s">
+        <v>115</v>
+      </c>
+      <c r="H26" s="12"/>
+    </row>
+    <row r="27" spans="1:8" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A27" s="15" t="s">
         <v>116</v>
-      </c>
-      <c r="H26" s="12"/>
-    </row>
-    <row r="27" spans="1:8" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A27" s="16" t="s">
-        <v>117</v>
       </c>
       <c r="B27" s="7"/>
       <c r="C27" s="12" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
       <c r="D27" s="12" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
       <c r="E27" s="12" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
       <c r="F27" s="12" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
       <c r="G27" s="12" t="s">
-        <v>118</v>
+        <v>117</v>
       </c>
       <c r="H27" s="12"/>
     </row>
@@ -30641,7 +30642,7 @@
 </file>
 
 <file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0300-000000000000}">
   <dimension ref="A1:C1000"/>
   <sheetViews>
     <sheetView workbookViewId="0"/>
@@ -30656,64 +30657,64 @@
   <sheetData>
     <row r="1" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A1" s="7" t="s">
+        <v>10</v>
+      </c>
+      <c r="B1" s="7" t="s">
         <v>11</v>
-      </c>
-      <c r="B1" s="7" t="s">
-        <v>12</v>
       </c>
     </row>
     <row r="2" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A2" s="7" t="s">
+        <v>12</v>
+      </c>
+      <c r="B2" s="7" t="s">
         <v>13</v>
-      </c>
-      <c r="B2" s="7" t="s">
-        <v>14</v>
       </c>
     </row>
     <row r="3" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A3" s="7" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="B3" s="7" t="s">
-        <v>119</v>
+        <v>118</v>
       </c>
     </row>
     <row r="4" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A4" s="7" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
     </row>
     <row r="5" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A5" s="7" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
       <c r="B5" s="7" t="s">
-        <v>120</v>
+        <v>119</v>
       </c>
     </row>
     <row r="6" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A6" s="7" t="s">
+        <v>19</v>
+      </c>
+      <c r="B6" s="7" t="s">
         <v>20</v>
-      </c>
-      <c r="B6" s="7" t="s">
-        <v>21</v>
       </c>
     </row>
     <row r="7" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A7" s="7" t="s">
+        <v>21</v>
+      </c>
+      <c r="B7" s="8" t="s">
         <v>22</v>
-      </c>
-      <c r="B7" s="8" t="s">
-        <v>23</v>
       </c>
       <c r="C7" s="9"/>
     </row>
     <row r="8" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A8" s="7" t="s">
+        <v>23</v>
+      </c>
+      <c r="B8" s="10" t="s">
         <v>24</v>
-      </c>
-      <c r="B8" s="10" t="s">
-        <v>25</v>
       </c>
     </row>
     <row r="21" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
@@ -31703,12 +31704,12 @@
 </file>
 
 <file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0400-000000000000}">
   <dimension ref="A1:I1000"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <pane xSplit="1" topLeftCell="B1" activePane="topRight" state="frozen"/>
-      <selection pane="topRight" activeCell="B9" sqref="B9"/>
+      <selection pane="topRight" activeCell="B8" sqref="B8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="14.42578125" defaultRowHeight="15" customHeight="1" x14ac:dyDescent="0.25"/>
@@ -31725,511 +31726,511 @@
   <sheetData>
     <row r="1" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A1" s="11" t="s">
+        <v>196</v>
+      </c>
+      <c r="B1" s="11" t="s">
         <v>197</v>
       </c>
-      <c r="B1" s="11" t="s">
-        <v>198</v>
-      </c>
       <c r="C1" s="11" t="s">
+        <v>25</v>
+      </c>
+      <c r="D1" s="11" t="s">
         <v>26</v>
       </c>
-      <c r="D1" s="11" t="s">
+      <c r="E1" s="11" t="s">
         <v>27</v>
       </c>
-      <c r="E1" s="11" t="s">
+      <c r="F1" s="11" t="s">
         <v>28</v>
       </c>
-      <c r="F1" s="11" t="s">
+      <c r="G1" s="11" t="s">
         <v>29</v>
       </c>
-      <c r="G1" s="11" t="s">
+      <c r="H1" s="11" t="s">
         <v>30</v>
       </c>
-      <c r="H1" s="11" t="s">
-        <v>31</v>
-      </c>
       <c r="I1" s="11" t="s">
-        <v>219</v>
+        <v>218</v>
       </c>
     </row>
     <row r="2" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A2" s="7" t="s">
+        <v>31</v>
+      </c>
+      <c r="B2" t="s">
+        <v>198</v>
+      </c>
+      <c r="C2" s="12" t="s">
         <v>32</v>
       </c>
-      <c r="B2" s="15" t="s">
-        <v>199</v>
-      </c>
-      <c r="C2" s="12" t="s">
+      <c r="D2" s="12" t="s">
         <v>33</v>
-      </c>
-      <c r="D2" s="12" t="s">
-        <v>34</v>
       </c>
       <c r="E2" s="12"/>
       <c r="F2" s="12" t="s">
+        <v>35</v>
+      </c>
+      <c r="G2" s="12" t="s">
         <v>36</v>
-      </c>
-      <c r="G2" s="12" t="s">
-        <v>37</v>
       </c>
       <c r="H2" s="12"/>
     </row>
     <row r="3" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A3" s="13" t="s">
+        <v>120</v>
+      </c>
+      <c r="B3" s="13" t="s">
+        <v>220</v>
+      </c>
+      <c r="C3" s="12" t="s">
         <v>121</v>
       </c>
-      <c r="B3" s="13" t="s">
-        <v>221</v>
-      </c>
-      <c r="C3" s="12" t="s">
+      <c r="D3" s="12" t="s">
+        <v>71</v>
+      </c>
+      <c r="E3" s="12" t="s">
         <v>122</v>
-      </c>
-      <c r="D3" s="12" t="s">
-        <v>72</v>
-      </c>
-      <c r="E3" s="12" t="s">
-        <v>123</v>
       </c>
       <c r="F3" s="12" t="s">
         <v>1</v>
       </c>
       <c r="G3" s="12" t="s">
-        <v>124</v>
+        <v>123</v>
       </c>
       <c r="H3" s="12"/>
     </row>
     <row r="4" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A4" s="13" t="s">
-        <v>125</v>
+        <v>124</v>
       </c>
       <c r="B4" s="13" t="s">
-        <v>222</v>
+        <v>221</v>
       </c>
       <c r="C4" s="12" t="s">
+        <v>38</v>
+      </c>
+      <c r="D4" s="12" t="s">
         <v>39</v>
-      </c>
-      <c r="D4" s="12" t="s">
-        <v>40</v>
       </c>
       <c r="E4" s="12"/>
       <c r="F4" s="12" t="s">
         <v>1</v>
       </c>
       <c r="G4" s="12" t="s">
-        <v>41</v>
+        <v>40</v>
       </c>
       <c r="H4" s="12"/>
     </row>
     <row r="5" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A5" s="13" t="s">
-        <v>126</v>
+        <v>125</v>
       </c>
       <c r="B5" s="13" t="s">
-        <v>223</v>
+        <v>222</v>
       </c>
       <c r="C5" s="12" t="s">
-        <v>43</v>
+        <v>42</v>
       </c>
       <c r="D5" s="12" t="s">
-        <v>40</v>
+        <v>39</v>
       </c>
       <c r="E5" s="12"/>
       <c r="F5" s="12" t="s">
         <v>1</v>
       </c>
       <c r="G5" s="12" t="s">
-        <v>44</v>
+        <v>43</v>
       </c>
       <c r="H5" s="12"/>
     </row>
     <row r="6" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A6" s="13" t="s">
+        <v>44</v>
+      </c>
+      <c r="B6" s="13" t="s">
+        <v>248</v>
+      </c>
+      <c r="C6" s="12" t="s">
         <v>45</v>
       </c>
-      <c r="B6" s="13" t="s">
-        <v>226</v>
-      </c>
-      <c r="C6" s="12" t="s">
+      <c r="D6" s="12" t="s">
         <v>46</v>
-      </c>
-      <c r="D6" s="12" t="s">
-        <v>47</v>
       </c>
       <c r="E6" s="12"/>
       <c r="F6" s="12" t="s">
+        <v>47</v>
+      </c>
+      <c r="G6" s="12" t="s">
         <v>48</v>
       </c>
-      <c r="G6" s="12" t="s">
+      <c r="H6" s="12" t="s">
         <v>49</v>
-      </c>
-      <c r="H6" s="12" t="s">
-        <v>50</v>
       </c>
     </row>
     <row r="7" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A7" s="13" t="s">
+        <v>50</v>
+      </c>
+      <c r="B7" s="13" t="s">
+        <v>249</v>
+      </c>
+      <c r="C7" s="12" t="s">
         <v>51</v>
       </c>
-      <c r="B7" s="13" t="s">
-        <v>227</v>
-      </c>
-      <c r="C7" s="12" t="s">
-        <v>52</v>
-      </c>
       <c r="D7" s="12" t="s">
-        <v>47</v>
+        <v>46</v>
       </c>
       <c r="E7" s="12"/>
       <c r="F7" s="12" t="s">
-        <v>48</v>
+        <v>47</v>
       </c>
       <c r="G7" s="12" t="s">
-        <v>53</v>
+        <v>52</v>
       </c>
       <c r="H7" s="12" t="s">
-        <v>50</v>
+        <v>49</v>
       </c>
     </row>
     <row r="8" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A8" s="13" t="s">
-        <v>54</v>
+        <v>53</v>
       </c>
       <c r="B8" s="13" t="s">
-        <v>246</v>
+        <v>241</v>
       </c>
       <c r="C8" s="12" t="s">
-        <v>127</v>
+        <v>126</v>
       </c>
       <c r="D8" s="12" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
       <c r="E8" s="12"/>
       <c r="F8" s="12" t="s">
         <v>1</v>
       </c>
       <c r="G8" s="12" t="s">
+        <v>55</v>
+      </c>
+      <c r="H8" s="12" t="s">
         <v>56</v>
-      </c>
-      <c r="H8" s="12" t="s">
-        <v>57</v>
       </c>
     </row>
     <row r="9" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A9" s="13" t="s">
-        <v>58</v>
+        <v>57</v>
       </c>
       <c r="B9" s="13" t="s">
-        <v>228</v>
+        <v>223</v>
       </c>
       <c r="C9" s="12" t="s">
-        <v>128</v>
+        <v>127</v>
       </c>
       <c r="D9" s="12" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
       <c r="E9" s="12"/>
       <c r="F9" s="12" t="s">
         <v>1</v>
       </c>
       <c r="G9" s="12" t="s">
-        <v>60</v>
+        <v>59</v>
       </c>
       <c r="H9" s="12" t="s">
-        <v>57</v>
+        <v>56</v>
       </c>
     </row>
     <row r="10" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A10" s="13" t="s">
-        <v>61</v>
+        <v>60</v>
       </c>
       <c r="B10" s="13" t="s">
-        <v>229</v>
+        <v>224</v>
       </c>
       <c r="C10" s="12" t="s">
-        <v>129</v>
+        <v>128</v>
       </c>
       <c r="D10" s="12" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
       <c r="E10" s="12"/>
       <c r="F10" s="12" t="s">
         <v>1</v>
       </c>
       <c r="G10" s="12" t="s">
-        <v>63</v>
+        <v>62</v>
       </c>
       <c r="H10" s="12"/>
     </row>
     <row r="11" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A11" s="13" t="s">
+        <v>129</v>
+      </c>
+      <c r="B11" s="13" t="s">
+        <v>225</v>
+      </c>
+      <c r="C11" s="12" t="s">
         <v>130</v>
       </c>
-      <c r="B11" s="13" t="s">
-        <v>230</v>
-      </c>
-      <c r="C11" s="19" t="s">
-        <v>131</v>
-      </c>
       <c r="D11" s="12" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
       <c r="E11" s="12"/>
       <c r="F11" s="12" t="s">
         <v>1</v>
       </c>
       <c r="G11" s="12" t="s">
-        <v>132</v>
+        <v>131</v>
       </c>
       <c r="H11" s="12"/>
     </row>
     <row r="12" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A12" s="13" t="s">
+        <v>132</v>
+      </c>
+      <c r="B12" s="13" t="s">
+        <v>226</v>
+      </c>
+      <c r="C12" s="12" t="s">
         <v>133</v>
       </c>
-      <c r="B12" s="13" t="s">
-        <v>231</v>
-      </c>
-      <c r="C12" s="19" t="s">
-        <v>134</v>
-      </c>
       <c r="D12" s="12" t="s">
+        <v>71</v>
+      </c>
+      <c r="E12" s="12" t="s">
         <v>72</v>
-      </c>
-      <c r="E12" s="12" t="s">
-        <v>73</v>
       </c>
       <c r="F12" s="12" t="s">
         <v>1</v>
       </c>
       <c r="G12" s="12" t="s">
-        <v>135</v>
+        <v>134</v>
       </c>
       <c r="H12" s="12"/>
     </row>
     <row r="13" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A13" s="13" t="s">
-        <v>76</v>
+        <v>75</v>
       </c>
       <c r="B13" s="13" t="s">
-        <v>232</v>
-      </c>
-      <c r="C13" s="19" t="s">
-        <v>136</v>
+        <v>227</v>
+      </c>
+      <c r="C13" s="12" t="s">
+        <v>135</v>
       </c>
       <c r="D13" s="12" t="s">
+        <v>71</v>
+      </c>
+      <c r="E13" s="12" t="s">
         <v>72</v>
-      </c>
-      <c r="E13" s="12" t="s">
-        <v>73</v>
       </c>
       <c r="F13" s="12" t="s">
         <v>1</v>
       </c>
       <c r="G13" s="12" t="s">
-        <v>137</v>
+        <v>136</v>
       </c>
       <c r="H13" s="12"/>
     </row>
     <row r="14" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A14" s="13" t="s">
+        <v>137</v>
+      </c>
+      <c r="B14" s="13" t="s">
+        <v>228</v>
+      </c>
+      <c r="C14" s="12" t="s">
         <v>138</v>
       </c>
-      <c r="B14" s="13" t="s">
-        <v>233</v>
-      </c>
-      <c r="C14" s="19" t="s">
-        <v>139</v>
-      </c>
       <c r="D14" s="12" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
       <c r="E14" s="12"/>
       <c r="F14" s="12" t="s">
         <v>1</v>
       </c>
       <c r="G14" s="12" t="s">
+        <v>139</v>
+      </c>
+      <c r="H14" s="12"/>
+    </row>
+    <row r="15" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A15" s="16" t="s">
         <v>140</v>
       </c>
-      <c r="H14" s="12"/>
-    </row>
-    <row r="15" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A15" s="17" t="s">
+      <c r="B15" s="13" t="s">
+        <v>229</v>
+      </c>
+      <c r="C15" s="17" t="s">
         <v>141</v>
       </c>
-      <c r="B15" s="13" t="s">
-        <v>234</v>
-      </c>
-      <c r="C15" s="18" t="s">
-        <v>142</v>
-      </c>
       <c r="D15" s="12" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
       <c r="E15" s="12"/>
       <c r="F15" s="12" t="s">
         <v>1</v>
       </c>
       <c r="G15" s="12" t="s">
+        <v>142</v>
+      </c>
+      <c r="H15" s="12" t="s">
+        <v>74</v>
+      </c>
+    </row>
+    <row r="16" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A16" s="16" t="s">
         <v>143</v>
       </c>
-      <c r="H15" s="12" t="s">
-        <v>75</v>
-      </c>
-    </row>
-    <row r="16" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A16" s="17" t="s">
+      <c r="B16" s="13" t="s">
+        <v>230</v>
+      </c>
+      <c r="C16" s="17" t="s">
         <v>144</v>
       </c>
-      <c r="B16" s="13" t="s">
-        <v>235</v>
-      </c>
-      <c r="C16" s="18" t="s">
-        <v>145</v>
-      </c>
       <c r="D16" s="12" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
       <c r="E16" s="12"/>
       <c r="F16" s="12" t="s">
         <v>1</v>
       </c>
       <c r="G16" s="12" t="s">
-        <v>146</v>
+        <v>145</v>
       </c>
       <c r="H16" s="12" t="s">
-        <v>75</v>
+        <v>74</v>
       </c>
     </row>
     <row r="17" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A17" s="13" t="s">
-        <v>70</v>
+        <v>69</v>
       </c>
       <c r="B17" s="13" t="s">
-        <v>206</v>
-      </c>
-      <c r="C17" s="19" t="s">
-        <v>147</v>
+        <v>205</v>
+      </c>
+      <c r="C17" s="12" t="s">
+        <v>146</v>
       </c>
       <c r="D17" s="12" t="s">
+        <v>71</v>
+      </c>
+      <c r="E17" s="12" t="s">
         <v>72</v>
-      </c>
-      <c r="E17" s="12" t="s">
-        <v>73</v>
       </c>
       <c r="F17" s="12" t="s">
         <v>1</v>
       </c>
       <c r="G17" s="12" t="s">
-        <v>74</v>
+        <v>73</v>
       </c>
       <c r="H17" s="12"/>
     </row>
     <row r="18" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A18" s="13" t="s">
+        <v>147</v>
+      </c>
+      <c r="B18" s="13" t="s">
+        <v>206</v>
+      </c>
+      <c r="C18" s="12" t="s">
         <v>148</v>
       </c>
-      <c r="B18" s="13" t="s">
-        <v>207</v>
-      </c>
-      <c r="C18" s="12" t="s">
-        <v>149</v>
-      </c>
       <c r="D18" s="12" t="s">
+        <v>71</v>
+      </c>
+      <c r="E18" s="12" t="s">
         <v>72</v>
-      </c>
-      <c r="E18" s="12" t="s">
-        <v>73</v>
       </c>
       <c r="F18" s="12" t="s">
         <v>1</v>
       </c>
       <c r="G18" s="12" t="s">
-        <v>150</v>
+        <v>149</v>
       </c>
       <c r="H18" s="12"/>
     </row>
     <row r="19" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A19" s="13" t="s">
-        <v>79</v>
+        <v>78</v>
       </c>
       <c r="B19" s="13" t="s">
-        <v>208</v>
+        <v>207</v>
       </c>
       <c r="C19" s="12" t="s">
-        <v>151</v>
+        <v>150</v>
       </c>
       <c r="D19" s="12" t="s">
+        <v>71</v>
+      </c>
+      <c r="E19" s="12" t="s">
         <v>72</v>
-      </c>
-      <c r="E19" s="12" t="s">
-        <v>73</v>
       </c>
       <c r="F19" s="12" t="s">
         <v>1</v>
       </c>
       <c r="G19" s="12" t="s">
-        <v>152</v>
+        <v>151</v>
       </c>
       <c r="H19" s="12"/>
     </row>
     <row r="20" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A20" s="13" t="s">
-        <v>82</v>
+        <v>81</v>
       </c>
       <c r="B20" s="13" t="s">
-        <v>209</v>
+        <v>208</v>
       </c>
       <c r="C20" s="12" t="s">
-        <v>153</v>
+        <v>152</v>
       </c>
       <c r="D20" s="12" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
       <c r="E20" s="12"/>
       <c r="F20" s="12" t="s">
         <v>1</v>
       </c>
       <c r="G20" s="12" t="s">
-        <v>154</v>
+        <v>153</v>
       </c>
       <c r="H20" s="12"/>
     </row>
     <row r="21" spans="1:9" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A21" s="13" t="s">
+        <v>154</v>
+      </c>
+      <c r="B21" s="13" t="s">
+        <v>234</v>
+      </c>
+      <c r="C21" s="12" t="s">
         <v>155</v>
       </c>
-      <c r="B21" s="13" t="s">
-        <v>239</v>
-      </c>
-      <c r="C21" s="12" t="s">
-        <v>156</v>
-      </c>
       <c r="D21" s="12" t="s">
+        <v>71</v>
+      </c>
+      <c r="E21" s="12" t="s">
         <v>72</v>
-      </c>
-      <c r="E21" s="12" t="s">
-        <v>73</v>
       </c>
       <c r="F21" s="12" t="s">
         <v>1</v>
       </c>
       <c r="G21" s="12" t="s">
-        <v>157</v>
+        <v>156</v>
       </c>
       <c r="H21" s="12"/>
     </row>
     <row r="22" spans="1:9" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A22" s="13" t="s">
+        <v>157</v>
+      </c>
+      <c r="B22" s="13" t="s">
+        <v>233</v>
+      </c>
+      <c r="C22" s="12" t="s">
         <v>158</v>
       </c>
-      <c r="B22" s="13" t="s">
-        <v>238</v>
-      </c>
-      <c r="C22" s="12" t="s">
-        <v>159</v>
-      </c>
       <c r="D22" s="12" t="s">
-        <v>47</v>
+        <v>46</v>
       </c>
       <c r="E22" s="12"/>
       <c r="F22" s="12" t="s">
@@ -32242,62 +32243,62 @@
     </row>
     <row r="23" spans="1:9" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A23" s="13" t="s">
-        <v>160</v>
+        <v>159</v>
       </c>
       <c r="B23" s="13" t="s">
-        <v>236</v>
+        <v>231</v>
       </c>
       <c r="C23" s="12" t="s">
-        <v>249</v>
-      </c>
-      <c r="D23" s="18" t="s">
-        <v>47</v>
+        <v>244</v>
+      </c>
+      <c r="D23" s="17" t="s">
+        <v>46</v>
       </c>
       <c r="E23" s="12"/>
       <c r="F23" s="12" t="s">
         <v>1</v>
       </c>
       <c r="G23" s="12" t="s">
-        <v>161</v>
+        <v>160</v>
       </c>
       <c r="H23" s="12"/>
     </row>
     <row r="24" spans="1:9" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A24" s="13" t="s">
-        <v>92</v>
+        <v>91</v>
       </c>
       <c r="B24" s="13" t="s">
-        <v>213</v>
+        <v>212</v>
       </c>
       <c r="C24" s="12" t="s">
-        <v>162</v>
+        <v>161</v>
       </c>
       <c r="D24" s="12" t="s">
+        <v>71</v>
+      </c>
+      <c r="E24" s="12" t="s">
         <v>72</v>
-      </c>
-      <c r="E24" s="12" t="s">
-        <v>73</v>
       </c>
       <c r="F24" s="12" t="s">
         <v>1</v>
       </c>
       <c r="G24" s="12" t="s">
-        <v>94</v>
+        <v>93</v>
       </c>
       <c r="H24" s="12"/>
     </row>
     <row r="25" spans="1:9" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A25" s="13" t="s">
-        <v>85</v>
+        <v>84</v>
       </c>
       <c r="B25" s="13" t="s">
-        <v>210</v>
+        <v>209</v>
       </c>
       <c r="C25" s="12" t="s">
-        <v>163</v>
+        <v>162</v>
       </c>
       <c r="D25" s="12" t="s">
-        <v>47</v>
+        <v>46</v>
       </c>
       <c r="E25" s="12"/>
       <c r="F25" s="12" t="s">
@@ -32310,16 +32311,16 @@
     </row>
     <row r="26" spans="1:9" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A26" s="13" t="s">
-        <v>88</v>
+        <v>87</v>
       </c>
       <c r="B26" s="13" t="s">
-        <v>211</v>
+        <v>210</v>
       </c>
       <c r="C26" s="12" t="s">
-        <v>164</v>
+        <v>163</v>
       </c>
       <c r="D26" s="12" t="s">
-        <v>47</v>
+        <v>46</v>
       </c>
       <c r="E26" s="12"/>
       <c r="F26" s="12" t="s">
@@ -32332,16 +32333,16 @@
     </row>
     <row r="27" spans="1:9" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A27" s="13" t="s">
-        <v>90</v>
+        <v>89</v>
       </c>
       <c r="B27" s="13" t="s">
-        <v>237</v>
+        <v>232</v>
       </c>
       <c r="C27" s="12" t="s">
-        <v>165</v>
+        <v>164</v>
       </c>
       <c r="D27" s="12" t="s">
-        <v>47</v>
+        <v>46</v>
       </c>
       <c r="E27" s="12"/>
       <c r="F27" s="12" t="s">
@@ -32354,311 +32355,311 @@
     </row>
     <row r="28" spans="1:9" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A28" s="13" t="s">
-        <v>95</v>
+        <v>94</v>
       </c>
       <c r="B28" s="13" t="s">
-        <v>214</v>
+        <v>213</v>
       </c>
       <c r="C28" s="12" t="s">
-        <v>166</v>
+        <v>165</v>
       </c>
       <c r="D28" s="12" t="s">
+        <v>71</v>
+      </c>
+      <c r="E28" s="12" t="s">
         <v>72</v>
-      </c>
-      <c r="E28" s="12" t="s">
-        <v>73</v>
       </c>
       <c r="F28" s="12" t="s">
         <v>1</v>
       </c>
       <c r="G28" s="12" t="s">
+        <v>166</v>
+      </c>
+      <c r="H28" s="12"/>
+    </row>
+    <row r="29" spans="1:9" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A29" s="16" t="s">
         <v>167</v>
       </c>
-      <c r="H28" s="12"/>
-    </row>
-    <row r="29" spans="1:9" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A29" s="17" t="s">
+      <c r="B29" s="13" t="s">
+        <v>235</v>
+      </c>
+      <c r="C29" s="12" t="s">
         <v>168</v>
       </c>
-      <c r="B29" s="13" t="s">
-        <v>240</v>
-      </c>
-      <c r="C29" s="12" t="s">
-        <v>169</v>
-      </c>
-      <c r="D29" s="18" t="s">
+      <c r="D29" s="17" t="s">
+        <v>71</v>
+      </c>
+      <c r="E29" s="12" t="s">
         <v>72</v>
-      </c>
-      <c r="E29" s="12" t="s">
-        <v>73</v>
       </c>
       <c r="F29" s="12" t="s">
         <v>1</v>
       </c>
       <c r="G29" s="12" t="s">
+        <v>169</v>
+      </c>
+      <c r="H29" s="12" t="s">
         <v>170</v>
       </c>
-      <c r="H29" s="12" t="s">
-        <v>171</v>
-      </c>
       <c r="I29" s="12" t="s">
-        <v>220</v>
+        <v>219</v>
       </c>
     </row>
     <row r="30" spans="1:9" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A30" s="13" t="s">
+        <v>171</v>
+      </c>
+      <c r="B30" s="13" t="s">
+        <v>236</v>
+      </c>
+      <c r="C30" s="12" t="s">
         <v>172</v>
       </c>
-      <c r="B30" s="13" t="s">
-        <v>241</v>
-      </c>
-      <c r="C30" s="12" t="s">
-        <v>173</v>
-      </c>
-      <c r="D30" s="19" t="s">
-        <v>47</v>
+      <c r="D30" s="12" t="s">
+        <v>46</v>
       </c>
       <c r="E30" s="12"/>
       <c r="F30" s="12" t="s">
         <v>1</v>
       </c>
       <c r="G30" s="12" t="s">
+        <v>173</v>
+      </c>
+      <c r="H30" s="12"/>
+    </row>
+    <row r="31" spans="1:9" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A31" s="16" t="s">
         <v>174</v>
       </c>
-      <c r="H30" s="12"/>
-    </row>
-    <row r="31" spans="1:9" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A31" s="17" t="s">
+      <c r="B31" s="13" t="s">
+        <v>237</v>
+      </c>
+      <c r="C31" s="12" t="s">
         <v>175</v>
       </c>
-      <c r="B31" s="13" t="s">
-        <v>242</v>
-      </c>
-      <c r="C31" s="12" t="s">
+      <c r="D31" s="12" t="s">
+        <v>71</v>
+      </c>
+      <c r="E31" s="12" t="s">
         <v>176</v>
-      </c>
-      <c r="D31" s="19" t="s">
-        <v>72</v>
-      </c>
-      <c r="E31" s="12" t="s">
-        <v>177</v>
       </c>
       <c r="F31" s="12" t="s">
         <v>1</v>
       </c>
       <c r="G31" s="12" t="s">
-        <v>178</v>
+        <v>177</v>
       </c>
       <c r="H31" s="12" t="s">
-        <v>171</v>
+        <v>170</v>
       </c>
       <c r="I31" s="12" t="s">
-        <v>220</v>
+        <v>219</v>
       </c>
     </row>
     <row r="32" spans="1:9" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A32" s="13" t="s">
-        <v>111</v>
+        <v>110</v>
       </c>
       <c r="B32" s="13" t="s">
-        <v>218</v>
+        <v>217</v>
       </c>
       <c r="C32" s="12" t="s">
-        <v>179</v>
+        <v>178</v>
       </c>
       <c r="D32" s="12" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
       <c r="E32" s="12"/>
       <c r="F32" s="12" t="s">
         <v>1</v>
       </c>
       <c r="G32" s="12" t="s">
-        <v>113</v>
+        <v>112</v>
       </c>
       <c r="H32" s="12"/>
     </row>
     <row r="33" spans="1:8" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A33" s="13" t="s">
-        <v>114</v>
+        <v>113</v>
       </c>
       <c r="B33" s="13" t="s">
-        <v>243</v>
+        <v>238</v>
       </c>
       <c r="C33" s="12" t="s">
-        <v>180</v>
+        <v>179</v>
       </c>
       <c r="D33" s="12" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
       <c r="E33" s="12"/>
       <c r="F33" s="12" t="s">
         <v>1</v>
       </c>
       <c r="G33" s="12" t="s">
-        <v>116</v>
+        <v>115</v>
       </c>
       <c r="H33" s="12"/>
     </row>
     <row r="34" spans="1:8" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A34" s="17" t="s">
+      <c r="A34" s="16" t="s">
+        <v>180</v>
+      </c>
+      <c r="B34" s="13" t="s">
+        <v>239</v>
+      </c>
+      <c r="C34" s="12" t="s">
         <v>181</v>
       </c>
-      <c r="B34" s="13" t="s">
-        <v>244</v>
-      </c>
-      <c r="C34" s="12" t="s">
-        <v>182</v>
-      </c>
       <c r="D34" s="12" t="s">
+        <v>71</v>
+      </c>
+      <c r="E34" s="12" t="s">
         <v>72</v>
-      </c>
-      <c r="E34" s="12" t="s">
-        <v>73</v>
       </c>
       <c r="F34" s="12" t="s">
         <v>1</v>
       </c>
       <c r="G34" s="12" t="s">
-        <v>183</v>
+        <v>182</v>
       </c>
       <c r="H34" s="12"/>
     </row>
     <row r="35" spans="1:8" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A35" s="13" t="s">
+        <v>183</v>
+      </c>
+      <c r="B35" s="13" t="s">
+        <v>240</v>
+      </c>
+      <c r="C35" s="12" t="s">
         <v>184</v>
       </c>
-      <c r="B35" s="13" t="s">
-        <v>245</v>
-      </c>
-      <c r="C35" s="12" t="s">
-        <v>185</v>
-      </c>
       <c r="D35" s="12" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
       <c r="E35" s="12"/>
       <c r="F35" s="12" t="s">
         <v>1</v>
       </c>
       <c r="G35" s="12" t="s">
+        <v>185</v>
+      </c>
+      <c r="H35" s="12"/>
+    </row>
+    <row r="36" spans="1:8" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A36" s="16" t="s">
+        <v>97</v>
+      </c>
+      <c r="B36" s="13" t="s">
+        <v>214</v>
+      </c>
+      <c r="C36" s="12" t="s">
         <v>186</v>
       </c>
-      <c r="H35" s="12"/>
-    </row>
-    <row r="36" spans="1:8" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A36" s="17" t="s">
-        <v>98</v>
-      </c>
-      <c r="B36" s="13" t="s">
-        <v>215</v>
-      </c>
-      <c r="C36" s="12" t="s">
-        <v>187</v>
-      </c>
       <c r="D36" s="12" t="s">
+        <v>71</v>
+      </c>
+      <c r="E36" s="12" t="s">
         <v>72</v>
-      </c>
-      <c r="E36" s="12" t="s">
-        <v>73</v>
       </c>
       <c r="F36" s="12" t="s">
         <v>1</v>
       </c>
       <c r="G36" s="12" t="s">
-        <v>188</v>
+        <v>187</v>
       </c>
       <c r="H36" s="12"/>
     </row>
     <row r="37" spans="1:8" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A37" s="13" t="s">
+        <v>188</v>
+      </c>
+      <c r="B37" s="13" t="s">
+        <v>243</v>
+      </c>
+      <c r="C37" s="12" t="s">
         <v>189</v>
       </c>
-      <c r="B37" s="13" t="s">
-        <v>248</v>
-      </c>
-      <c r="C37" s="12" t="s">
-        <v>190</v>
-      </c>
       <c r="D37" s="12" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
       <c r="E37" s="12"/>
       <c r="F37" s="12" t="s">
         <v>1</v>
       </c>
       <c r="G37" s="12" t="s">
-        <v>191</v>
+        <v>190</v>
       </c>
       <c r="H37" s="12" t="s">
-        <v>104</v>
+        <v>103</v>
       </c>
     </row>
     <row r="38" spans="1:8" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A38" s="13" t="s">
+        <v>191</v>
+      </c>
+      <c r="B38" s="13" t="s">
+        <v>223</v>
+      </c>
+      <c r="C38" s="12" t="s">
         <v>192</v>
       </c>
-      <c r="B38" s="13" t="s">
-        <v>228</v>
-      </c>
-      <c r="C38" s="12" t="s">
-        <v>193</v>
-      </c>
       <c r="D38" s="12" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
       <c r="E38" s="12"/>
       <c r="F38" s="12" t="s">
         <v>1</v>
       </c>
       <c r="G38" s="12" t="s">
-        <v>194</v>
+        <v>193</v>
       </c>
       <c r="H38" s="12" t="s">
-        <v>57</v>
+        <v>56</v>
       </c>
     </row>
     <row r="39" spans="1:8" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A39" s="13" t="s">
-        <v>108</v>
+        <v>107</v>
       </c>
       <c r="B39" s="13" t="s">
-        <v>217</v>
+        <v>216</v>
       </c>
       <c r="C39" s="12" t="s">
-        <v>195</v>
+        <v>194</v>
       </c>
       <c r="D39" s="12" t="s">
-        <v>40</v>
+        <v>39</v>
       </c>
       <c r="E39" s="12"/>
       <c r="F39" s="12" t="s">
         <v>1</v>
       </c>
       <c r="G39" s="12" t="s">
-        <v>41</v>
+        <v>40</v>
       </c>
       <c r="H39" s="12"/>
     </row>
     <row r="40" spans="1:8" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A40" s="16" t="s">
-        <v>196</v>
+      <c r="A40" s="15" t="s">
+        <v>195</v>
       </c>
       <c r="B40" s="7"/>
       <c r="C40" s="12" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
       <c r="D40" s="12" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
       <c r="E40" s="12" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
       <c r="F40" s="12" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
       <c r="G40" s="12" t="s">
-        <v>118</v>
+        <v>117</v>
       </c>
       <c r="H40" s="12"/>
     </row>

</xml_diff>